<commit_message>
FIX: Adds correct alignment (#89)
</commit_message>
<xml_diff>
--- a/packages/calc/equalto_xlsx/tests/basic_text.xlsx
+++ b/packages/calc/equalto_xlsx/tests/basic_text.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nicolas/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{233BF6EC-3EA5-5B4D-9F5F-7840B7EAB7CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87BA770-0859-2C4B-A2E6-C005D0FF56F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{3E620F9E-FF5E-2B4D-93CE-B2116FA7EAA2}"/>
+    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{3E620F9E-FF5E-2B4D-93CE-B2116FA7EAA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="alignment" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Bold</t>
   </si>
@@ -66,6 +67,39 @@
   </si>
   <si>
     <t>Font size 24 px</t>
+  </si>
+  <si>
+    <t>Horizontal</t>
+  </si>
+  <si>
+    <t>Vertical</t>
+  </si>
+  <si>
+    <t>No alignment</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Distributed</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Center</t>
+  </si>
+  <si>
+    <t>Fill</t>
+  </si>
+  <si>
+    <t>Justify</t>
+  </si>
+  <si>
+    <t>Bottom</t>
+  </si>
+  <si>
+    <t>Top</t>
   </si>
 </sst>
 </file>
@@ -167,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -180,6 +214,36 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="distributed"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="distributed"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -496,7 +560,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC7B437E-E9AA-EC43-95BA-CBDE4C615940}">
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
@@ -548,4 +612,84 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E041BF07-E324-5C44-AF6F-8A006535C48E}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="32" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="39" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="42" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="55" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="59" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="56" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>